<commit_message>
menu bar and  bug fixes
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -471,25 +471,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fe</t>
+          <t>48</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>male@yahoo.com</t>
+          <t>4833@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>Realtime</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['#Europ']</t>
+          <t>['#Volunteering', '#YouthProjects', '#Career', '#Education']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added comments, and readme
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,126 +468,62 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1271736470</t>
+          <t>1771253784</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>hsbfj wfih</t>
+          <t>Անահիտ Մկրտչյան</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>hdfbcusab@gmail.com</t>
+          <t>anahitmkrtchyan658@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Realtime</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['#PersonalDevelopment', '#Leadership', '#Internships', '#Education']</t>
+          <t>['#Education', '#Internships', '#Workshops']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1393896015</t>
+          <t>1470163786</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>rrr</t>
+          <t>Նարե Զաքարյան</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>w@mail.ru</t>
+          <t>zakaryannare13@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Realtime</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t>['#Volunteering', '#Education', '#Career']</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1771253784</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Անահիտ Մկրտչյան</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>anahitmkrtchyan658@gmail.com</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>['#Education', '#Internships', '#Workshops']</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1470163786</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Նարե Զաքարյան</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>zakaryannare13@gmail.com</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>00:00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t>['#Leadership', '#Europ', '#Career']</t>
         </is>

</xml_diff>